<commit_message>
update units used in the utility tariff template.
</commit_message>
<xml_diff>
--- a/lib/btap/measures/UtilityTariffs/resources/utility_gas_tariffs.xlsx
+++ b/lib/btap/measures/UtilityTariffs/resources/utility_gas_tariffs.xlsx
@@ -81,16 +81,16 @@
     <t>Energy Charges Block 4 Limit (MJ)</t>
   </si>
   <si>
-    <t>Demand Charges Block 1 Limit (MJ)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 2 Limit (MJ)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 3 Limit (MJ)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 4 Limit (MJ)</t>
+    <t>Demand Charges Block 1 Limit (MW)</t>
+  </si>
+  <si>
+    <t>Demand Charges Block 2 Limit (MW)</t>
+  </si>
+  <si>
+    <t>Demand Charges Block 3 Limit (MW)</t>
+  </si>
+  <si>
+    <t>Demand Charges Block 4 Limit (MW)</t>
   </si>
 </sst>
 </file>
@@ -431,9 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>